<commit_message>
Correcion rutas metodos regla falsa,secante, lagrange y newtonint. Mejora de front para metodo regla falsa y secante
</commit_message>
<xml_diff>
--- a/app/tables/tabla_newtonint.xlsx
+++ b/app/tables/tabla_newtonint.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,12 +436,12 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
@@ -449,16 +449,38 @@
           <t>0</t>
         </is>
       </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>0.1</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>-1</v>
+        <v>4</v>
       </c>
       <c r="B2" t="n">
         <v>3</v>
       </c>
       <c r="C2" t="n">
-        <v>-0.5</v>
+        <v>1</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>6</v>
+      </c>
+      <c r="B3" t="n">
+        <v>5</v>
+      </c>
+      <c r="C3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>